<commit_message>
Spinks - Asset List, U bench update
</commit_message>
<xml_diff>
--- a/Documents/Archery Madness - Asset List - Secondary.xlsx
+++ b/Documents/Archery Madness - Asset List - Secondary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archery_Madness\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03129213-1183-42BD-9D00-71D3FFE788D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0338A8BE-B498-4EEF-979D-8DD5BF51BF55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>Button</t>
   </si>
   <si>
-    <t>Bench</t>
-  </si>
-  <si>
     <t>Quiver Textures</t>
   </si>
   <si>
@@ -120,10 +117,6 @@
   </si>
   <si>
     <t>Old Oak Wood</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -Is not actually a bench, It is more like a counter top.
- -This is a old, worn counter top, that has been polished over the years by the drinks/blood/sweat and tears of those who have been at this sideshow.</t>
   </si>
   <si>
     <t>Pirority</t>
@@ -152,6 +145,14 @@
  -Red- An image of a fire bird being doused by water
  -Green- Wood bird being punched by a boxing glove
  -Blue- A roman/greek helmet with a knife piercing through it.</t>
+  </si>
+  <si>
+    <t>U Bench</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Is not actually a bench, It is more like a counter top.
+ -This is a old, worn counter top, that has been polished over the years by the drinks/blood/sweat and tears of those who have been at this sideshow.
+ -This U bench needs to be able to accomadate a person sitting/standing in the middle of it.</t>
   </si>
 </sst>
 </file>
@@ -959,6 +960,50 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>244928</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4109357</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1076784</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E6C4597-8444-43DC-AA66-0EB50F8DE5B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4354285" y="10327821"/>
+          <a:ext cx="3864429" cy="967927"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1231,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1292,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1287,10 +1332,10 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1298,7 +1343,7 @@
     </row>
     <row r="5" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -1321,10 +1366,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="84.75" customHeight="1" x14ac:dyDescent="1.35">
@@ -1343,7 +1388,7 @@
     </row>
     <row r="9" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -1369,7 +1414,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="1.35">
@@ -1383,7 +1428,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="1.35">
@@ -1394,10 +1439,10 @@
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="1.35">
@@ -1405,13 +1450,13 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="1.35">
@@ -1419,13 +1464,13 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spinks - updated secondary asset list with fletching images
</commit_message>
<xml_diff>
--- a/Documents/Archery Madness - Asset List - Secondary.xlsx
+++ b/Documents/Archery Madness - Asset List - Secondary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archery_Madness\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0338A8BE-B498-4EEF-979D-8DD5BF51BF55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FA4878-3F5A-41C2-B066-2DEE282DCD14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1000,6 +1000,94 @@
         <a:xfrm>
           <a:off x="4354285" y="10327821"/>
           <a:ext cx="3864429" cy="967927"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>489857</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>575071</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>391679</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A676A379-ECB4-4D99-BE92-6FA8D201B213}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17349107" y="258536"/>
+          <a:ext cx="4085714" cy="1657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>204108</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>217714</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>446132</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1227238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A86A4F6-4E3E-4383-885E-49AFFE1A33D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21676179" y="476250"/>
+          <a:ext cx="1466667" cy="1009524"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1276,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>